<commit_message>
added dgs3mo and USD to Foreign Exchange rates
need to do insurance markets?
</commit_message>
<xml_diff>
--- a/code/Screener/data/interim/record.xlsx
+++ b/code/Screener/data/interim/record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\data\interim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E62F15-7226-4118-9CD3-BDDF75C41E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52CEF42-D122-4CCA-B83B-821F284D4AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="15" windowWidth="21870" windowHeight="12930" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Record book" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="1130">
   <si>
     <t>MCK</t>
   </si>
@@ -3456,13 +3456,19 @@
   </si>
   <si>
     <t>CSL</t>
+  </si>
+  <si>
+    <t>Funds</t>
+  </si>
+  <si>
+    <t>Sell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3542,7 +3548,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3570,7 +3594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3662,7 +3686,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5746,7 +5776,7 @@
   <dimension ref="A3:V45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5760,15 +5790,15 @@
     <col min="22" max="22" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="B3" t="s">
         <v>1120</v>
       </c>
       <c r="C3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="B4" t="s">
         <v>1121</v>
       </c>
@@ -5776,21 +5806,21 @@
         <v>44749</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:20">
       <c r="I9" s="19"/>
       <c r="K9">
         <f>SUM(K11:K30)</f>
-        <v>-7498.1300154999999</v>
+        <v>-9641.9300155000001</v>
       </c>
       <c r="N9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44751</v>
+        <v>44759</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="77.25">
+    <row r="10" spans="1:20" ht="77.25">
       <c r="A10" t="s">
         <v>1126</v>
       </c>
@@ -5843,8 +5873,11 @@
       <c r="S10" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="T10" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="1">
         <v>44749</v>
       </c>
@@ -5871,14 +5904,14 @@
         <v>308.74</v>
       </c>
       <c r="I11">
-        <f>G11*E11</f>
+        <f t="shared" ref="I11:I17" si="0">G11*E11</f>
         <v>971.09999999999991</v>
       </c>
       <c r="J11" s="19">
         <v>-1</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K11" si="0">J11*I11</f>
+        <f t="shared" ref="K11" si="1">J11*I11</f>
         <v>-971.09999999999991</v>
       </c>
       <c r="L11" t="s">
@@ -5891,158 +5924,158 @@
         <v>44832</v>
       </c>
       <c r="O11" s="28">
-        <f ca="1">$N$9-N11</f>
-        <v>-81</v>
+        <f t="shared" ref="O11:O17" ca="1" si="2">$N$9-N11</f>
+        <v>-73</v>
       </c>
       <c r="P11">
         <v>0.41</v>
       </c>
       <c r="Q11" s="16">
-        <f>N11-B11</f>
+        <f t="shared" ref="Q11:Q17" si="3">N11-B11</f>
         <v>83</v>
       </c>
       <c r="R11" s="16">
-        <f t="shared" ref="R11" si="1">(1+P11)^(1/Q11)-1</f>
+        <f t="shared" ref="R11" si="4">(1+P11)^(1/Q11)-1</f>
         <v>4.1482151170300074E-3</v>
       </c>
       <c r="S11" s="16">
-        <f t="shared" ref="S11:S12" si="2">(1+R11)^92</f>
+        <f t="shared" ref="S11:S12" si="5">(1+R11)^92</f>
         <v>1.4635228193247447</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="1">
+    <row r="12" spans="1:20" s="44" customFormat="1">
+      <c r="A12" s="48">
         <v>44749</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="48">
         <v>44749</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="30" t="s">
         <v>1104</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="30">
         <v>25</v>
       </c>
-      <c r="F12" s="39" cm="1">
+      <c r="F12" s="30" cm="1">
         <f t="array" ref="F12">SUMPRODUCT(($C$11:$C$32=C12)*($E$11:$E$32))</f>
-        <v>25</v>
-      </c>
-      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="G12" s="30">
         <v>43.41</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="30">
         <v>40.93</v>
       </c>
-      <c r="I12" s="39">
-        <f>G12*E12</f>
+      <c r="I12" s="30">
+        <f t="shared" si="0"/>
         <v>1085.25</v>
       </c>
-      <c r="J12" s="39">
+      <c r="J12" s="30">
         <v>-1</v>
       </c>
-      <c r="K12" s="39">
-        <f t="shared" ref="K12" si="3">J12*I12</f>
+      <c r="K12" s="30">
+        <f t="shared" ref="K12" si="6">J12*I12</f>
         <v>-1085.25</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="30" t="s">
         <v>1088</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="48">
         <v>44783</v>
       </c>
-      <c r="O12" s="28">
-        <f ca="1">$N$9-N12</f>
-        <v>-32</v>
-      </c>
-      <c r="P12">
+      <c r="O12" s="49">
+        <f t="shared" ca="1" si="2"/>
+        <v>-24</v>
+      </c>
+      <c r="P12" s="30">
         <v>0.10970000000000001</v>
       </c>
-      <c r="Q12" s="39">
-        <f>N12-B12</f>
+      <c r="Q12" s="30">
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="R12" s="39">
-        <f t="shared" ref="R12" si="4">(1+P12)^(1/Q12)-1</f>
+      <c r="R12" s="30">
+        <f t="shared" ref="R12" si="7">(1+P12)^(1/Q12)-1</f>
         <v>3.0661530762055023E-3</v>
       </c>
-      <c r="S12" s="39">
-        <f t="shared" si="2"/>
+      <c r="S12" s="30">
+        <f t="shared" si="5"/>
         <v>1.3253207497409916</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="1">
+    <row r="13" spans="1:20">
+      <c r="A13" s="48">
         <v>44750</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="48">
         <v>44751</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="30" t="s">
         <v>1122</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="30">
         <v>16</v>
       </c>
-      <c r="F13" s="39" cm="1">
+      <c r="F13" s="30" cm="1">
         <f t="array" ref="F13">SUMPRODUCT(($C$11:$C$32=C13)*($E$11:$E$32))</f>
         <v>16</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="30">
         <v>68</v>
       </c>
-      <c r="H13" s="39">
+      <c r="H13" s="30">
         <v>67.671330400000002</v>
       </c>
-      <c r="I13" s="39">
-        <f>G13*E13</f>
+      <c r="I13" s="30">
+        <f t="shared" si="0"/>
         <v>1088</v>
       </c>
-      <c r="J13" s="39">
+      <c r="J13" s="30">
         <v>-1</v>
       </c>
-      <c r="K13" s="39">
-        <f t="shared" ref="K13" si="5">J13*I13</f>
+      <c r="K13" s="30">
+        <f t="shared" ref="K13" si="8">J13*I13</f>
         <v>-1088</v>
       </c>
-      <c r="L13" s="39" t="s">
+      <c r="L13" s="30" t="s">
         <v>1088</v>
       </c>
-      <c r="M13" s="39" t="s">
+      <c r="M13" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N13" s="48">
         <v>44806</v>
       </c>
-      <c r="O13" s="28">
-        <f ca="1">$N$9-N13</f>
-        <v>-55</v>
-      </c>
-      <c r="P13" s="39">
+      <c r="O13" s="49">
+        <f t="shared" ca="1" si="2"/>
+        <v>-47</v>
+      </c>
+      <c r="P13" s="30">
         <v>0.10970000000000001</v>
       </c>
-      <c r="Q13" s="39">
-        <f>N13-B13</f>
+      <c r="Q13" s="30">
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
-      <c r="R13" s="39">
-        <f t="shared" ref="R13" si="6">(1+P13)^(1/Q13)-1</f>
+      <c r="R13" s="30">
+        <f t="shared" ref="R13" si="9">(1+P13)^(1/Q13)-1</f>
         <v>1.894332139396937E-3</v>
       </c>
-      <c r="S13" s="39">
-        <f t="shared" ref="S13" si="7">(1+R13)^92</f>
+      <c r="S13" s="30">
+        <f t="shared" ref="S13" si="10">(1+R13)^92</f>
         <v>1.1901908759978845</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:20">
       <c r="A14" s="1">
         <v>44750</v>
       </c>
@@ -6069,14 +6102,14 @@
         <v>83.34</v>
       </c>
       <c r="I14" s="39">
-        <f>G14*E14</f>
+        <f t="shared" si="0"/>
         <v>1063.08</v>
       </c>
       <c r="J14" s="39">
         <v>-1</v>
       </c>
       <c r="K14" s="39">
-        <f t="shared" ref="K14" si="8">J14*I14</f>
+        <f t="shared" ref="K14" si="11">J14*I14</f>
         <v>-1063.08</v>
       </c>
       <c r="L14" s="39" t="s">
@@ -6089,26 +6122,26 @@
         <v>44764</v>
       </c>
       <c r="O14" s="28">
-        <f ca="1">$N$9-N14</f>
-        <v>-13</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-5</v>
       </c>
       <c r="P14" s="39">
         <v>5.4993818E-2</v>
       </c>
       <c r="Q14" s="39">
-        <f>N14-B14</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="R14" s="39">
-        <f t="shared" ref="R14" si="9">(1+P14)^(1/Q14)-1</f>
+        <f t="shared" ref="R14" si="12">(1+P14)^(1/Q14)-1</f>
         <v>4.1265606849947289E-3</v>
       </c>
       <c r="S14" s="39">
-        <f t="shared" ref="S14" si="10">(1+R14)^92</f>
+        <f t="shared" ref="S14" si="13">(1+R14)^92</f>
         <v>1.4606220697552039</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20">
       <c r="A15" s="1">
         <v>44750</v>
       </c>
@@ -6135,14 +6168,14 @@
         <v>43.161925400000001</v>
       </c>
       <c r="I15">
-        <f>G15*E15</f>
+        <f t="shared" si="0"/>
         <v>997.5</v>
       </c>
       <c r="J15" s="39">
         <v>-1</v>
       </c>
       <c r="K15" s="39">
-        <f t="shared" ref="K15" si="11">J15*I15</f>
+        <f t="shared" ref="K15" si="14">J15*I15</f>
         <v>-997.5</v>
       </c>
       <c r="L15" s="39" t="s">
@@ -6155,26 +6188,26 @@
         <v>44827</v>
       </c>
       <c r="O15" s="28">
-        <f ca="1">$N$9-N15</f>
-        <v>-76</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-68</v>
       </c>
       <c r="P15" s="39">
         <v>0.271989859</v>
       </c>
       <c r="Q15" s="39">
-        <f>N15-B15</f>
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="R15" s="39">
-        <f t="shared" ref="R15" si="12">(1+P15)^(1/Q15)-1</f>
+        <f t="shared" ref="R15" si="15">(1+P15)^(1/Q15)-1</f>
         <v>3.1705747838659537E-3</v>
       </c>
       <c r="S15" s="39">
-        <f t="shared" ref="S15" si="13">(1+R15)^92</f>
+        <f t="shared" ref="S15" si="16">(1+R15)^92</f>
         <v>1.3380742295686983</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:20">
       <c r="A16" s="1">
         <v>44750</v>
       </c>
@@ -6192,7 +6225,7 @@
       </c>
       <c r="F16" s="19" cm="1">
         <f t="array" ref="F16">SUMPRODUCT(($C$11:$C$32=C16)*($E$11:$E$32))</f>
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="G16">
         <v>29.87</v>
@@ -6201,14 +6234,14 @@
         <v>28.318296019999998</v>
       </c>
       <c r="I16">
-        <f>G16*E16</f>
+        <f t="shared" si="0"/>
         <v>1045.45</v>
       </c>
       <c r="J16" s="39">
         <v>-1</v>
       </c>
       <c r="K16" s="39">
-        <f t="shared" ref="K16" si="14">J16*I16</f>
+        <f t="shared" ref="K16" si="17">J16*I16</f>
         <v>-1045.45</v>
       </c>
       <c r="L16" s="39" t="s">
@@ -6221,103 +6254,168 @@
         <v>44834</v>
       </c>
       <c r="O16" s="28">
-        <f ca="1">$N$9-N16</f>
-        <v>-83</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-75</v>
       </c>
       <c r="P16" s="39">
         <v>0.27529012899999999</v>
       </c>
       <c r="Q16" s="39">
-        <f>N16-B16</f>
+        <f t="shared" si="3"/>
         <v>83</v>
       </c>
       <c r="R16" s="39">
-        <f t="shared" ref="R16" si="15">(1+P16)^(1/Q16)-1</f>
+        <f t="shared" ref="R16" si="18">(1+P16)^(1/Q16)-1</f>
         <v>2.9340997425713056E-3</v>
       </c>
       <c r="S16" s="39">
-        <f t="shared" ref="S16" si="16">(1+R16)^92</f>
+        <f t="shared" ref="S16" si="19">(1+R16)^92</f>
         <v>1.3093645431271499</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
-      <c r="A17" s="1">
+    <row r="17" spans="1:20">
+      <c r="A17" s="43">
         <v>44750</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="43">
         <v>44751</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="44" t="s">
         <v>1127</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="44">
         <v>5</v>
       </c>
-      <c r="F17" s="19" cm="1">
+      <c r="F17" s="44" cm="1">
         <f t="array" ref="F17">SUMPRODUCT(($C$11:$C$32=C17)*($E$11:$E$32))</f>
         <v>5</v>
       </c>
-      <c r="G17" s="39">
+      <c r="G17" s="44">
         <v>249.5500031</v>
       </c>
-      <c r="H17" s="43">
+      <c r="H17" s="47">
         <v>246.35678720000001</v>
       </c>
-      <c r="I17">
-        <f>G17*E17</f>
+      <c r="I17" s="44">
+        <f t="shared" si="0"/>
         <v>1247.7500155</v>
       </c>
-      <c r="J17" s="39">
+      <c r="J17" s="44">
         <v>-1</v>
       </c>
-      <c r="K17" s="39">
-        <f t="shared" ref="K17" si="17">J17*I17</f>
+      <c r="K17" s="44">
+        <f t="shared" ref="K17:K19" si="20">J17*I17</f>
         <v>-1247.7500155</v>
       </c>
-      <c r="L17" s="39" t="s">
+      <c r="L17" s="44" t="s">
         <v>1088</v>
       </c>
-      <c r="M17" s="18" t="s">
+      <c r="M17" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N17" s="43">
         <v>44827</v>
       </c>
-      <c r="O17" s="28">
-        <f ca="1">$N$9-N17</f>
-        <v>-76</v>
-      </c>
-      <c r="P17" s="39">
+      <c r="O17" s="45">
+        <f t="shared" ca="1" si="2"/>
+        <v>-68</v>
+      </c>
+      <c r="P17" s="44">
         <v>0.142485214</v>
       </c>
-      <c r="Q17" s="39">
-        <f>N17-B17</f>
+      <c r="Q17" s="44">
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="R17" s="39">
-        <f t="shared" ref="R17" si="18">(1+P17)^(1/Q17)-1</f>
+      <c r="R17" s="44">
+        <f t="shared" ref="R17" si="21">(1+P17)^(1/Q17)-1</f>
         <v>1.7542461282435973E-3</v>
       </c>
-      <c r="S17" s="39">
-        <f t="shared" ref="S17" si="19">(1+R17)^92</f>
+      <c r="S17" s="44">
+        <f t="shared" ref="S17" si="22">(1+R17)^92</f>
         <v>1.1749777951563771</v>
       </c>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="B18" s="1"/>
-      <c r="J18" s="19"/>
+      <c r="T17">
+        <v>25193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="B18" s="1">
+        <v>44759</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E18">
+        <v>35</v>
+      </c>
+      <c r="F18" s="19" cm="1">
+        <f t="array" ref="F18">SUMPRODUCT(($C$11:$C$32=C18)*($E$11:$E$32))</f>
+        <v>70</v>
+      </c>
+      <c r="G18">
+        <v>29.33</v>
+      </c>
+      <c r="H18" s="47">
+        <v>246.35678720000001</v>
+      </c>
+      <c r="I18" s="44">
+        <f t="shared" ref="I18" si="23">G18*E18</f>
+        <v>1026.55</v>
+      </c>
+      <c r="J18" s="44">
+        <v>-1</v>
+      </c>
+      <c r="K18" s="44">
+        <f t="shared" si="20"/>
+        <v>-1026.55</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="28"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="18"/>
       <c r="S18" s="18"/>
     </row>
-    <row r="19" spans="1:19">
-      <c r="B19" s="1"/>
-      <c r="J19" s="19"/>
+    <row r="19" spans="1:20">
+      <c r="B19" s="1">
+        <v>44759</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E19">
+        <v>25</v>
+      </c>
+      <c r="F19" s="19" cm="1">
+        <f t="array" ref="F19">SUMPRODUCT(($C$11:$C$32=C19)*($E$11:$E$32))</f>
+        <v>50</v>
+      </c>
+      <c r="G19">
+        <v>44.69</v>
+      </c>
+      <c r="H19" s="47">
+        <v>246.35678720000001</v>
+      </c>
+      <c r="I19" s="44">
+        <f t="shared" ref="I19" si="24">G19*E19</f>
+        <v>1117.25</v>
+      </c>
+      <c r="J19" s="44">
+        <v>-1</v>
+      </c>
+      <c r="K19" s="44">
+        <f t="shared" si="20"/>
+        <v>-1117.25</v>
+      </c>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
       <c r="N19" s="1"/>
@@ -6327,7 +6425,7 @@
       <c r="R19" s="18"/>
       <c r="S19" s="18"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:20">
       <c r="B20" s="1"/>
       <c r="J20" s="19"/>
       <c r="L20" s="18"/>
@@ -6335,7 +6433,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="28"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:20">
       <c r="B21" s="1"/>
       <c r="J21" s="19"/>
       <c r="L21" s="18"/>
@@ -6347,7 +6445,7 @@
       <c r="R21" s="18"/>
       <c r="S21" s="18"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:20">
       <c r="B22" s="1"/>
       <c r="J22" s="19"/>
       <c r="L22" s="18"/>
@@ -6358,7 +6456,7 @@
       <c r="R22" s="18"/>
       <c r="S22" s="18"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:20">
       <c r="B23" s="1"/>
       <c r="J23" s="19"/>
       <c r="L23" s="18"/>
@@ -6369,7 +6467,7 @@
       <c r="R23" s="18"/>
       <c r="S23" s="18"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:20">
       <c r="B24" s="1"/>
       <c r="J24" s="19"/>
       <c r="L24" s="18"/>
@@ -6380,7 +6478,7 @@
       <c r="R24" s="18"/>
       <c r="S24" s="18"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:20">
       <c r="B25" s="1"/>
       <c r="D25" s="18"/>
       <c r="J25" s="19"/>
@@ -6394,7 +6492,7 @@
       <c r="R25" s="18"/>
       <c r="S25" s="18"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:20">
       <c r="B26" s="1"/>
       <c r="J26" s="19"/>
       <c r="L26" s="18"/>
@@ -6405,7 +6503,7 @@
       <c r="R26" s="18"/>
       <c r="S26" s="18"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:20">
       <c r="B27" s="1"/>
       <c r="D27" s="18"/>
       <c r="J27" s="19"/>
@@ -6418,7 +6516,7 @@
       <c r="R27" s="18"/>
       <c r="S27" s="18"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:20">
       <c r="B28" s="1"/>
       <c r="D28" s="18"/>
       <c r="J28" s="19"/>
@@ -6432,7 +6530,7 @@
       <c r="R28" s="18"/>
       <c r="S28" s="18"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:20">
       <c r="B29" s="1"/>
       <c r="D29" s="18"/>
       <c r="J29" s="19"/>
@@ -6446,7 +6544,7 @@
       <c r="R29" s="18"/>
       <c r="S29" s="18"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:20">
       <c r="B30" s="1"/>
       <c r="D30" s="18"/>
       <c r="J30" s="19"/>
@@ -6459,7 +6557,7 @@
       <c r="R30" s="18"/>
       <c r="S30" s="18"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:20">
       <c r="B31" s="1"/>
       <c r="J31" s="19"/>
       <c r="L31" s="18"/>
@@ -6470,7 +6568,7 @@
       <c r="R31" s="18"/>
       <c r="S31" s="18"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:20">
       <c r="B32" s="1"/>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>

</xml_diff>

<commit_message>
v14.11 correlation matrix cleaned up, outputs to a single excel file
</commit_message>
<xml_diff>
--- a/code/Screener/data/interim/record.xlsx
+++ b/code/Screener/data/interim/record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\data\interim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0A75DD-2AAB-4BA6-9A27-A7B8793EC796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFD1AF3-BDEE-40D2-B034-279556C81F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="-16830" windowWidth="23595" windowHeight="16200" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
+    <workbookView xWindow="4515" yWindow="-10770" windowWidth="20730" windowHeight="11835" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Record book" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1137">
   <si>
     <t>MCK</t>
   </si>
@@ -3459,6 +3459,30 @@
   </si>
   <si>
     <t>SCI</t>
+  </si>
+  <si>
+    <t>PGR</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>FHN</t>
+  </si>
+  <si>
+    <t>Login with</t>
+  </si>
+  <si>
+    <t>laferrierejc1</t>
+  </si>
+  <si>
+    <t>RGP</t>
+  </si>
+  <si>
+    <t>SP5600</t>
+  </si>
+  <si>
+    <t>Industrial</t>
   </si>
 </sst>
 </file>
@@ -3573,7 +3597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3659,6 +3683,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3666,7 +3692,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5750,14 +5775,14 @@
   <dimension ref="A3:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="18"/>
     <col min="8" max="8" width="9.140625" style="38"/>
     <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -5780,16 +5805,30 @@
       <c r="C4" s="1">
         <v>44766</v>
       </c>
+      <c r="E4" s="1">
+        <f ca="1">TODAY()</f>
+        <v>44772</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="D7" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="D8" t="s">
+        <v>1133</v>
+      </c>
     </row>
     <row r="9" spans="1:22">
       <c r="I9" s="18"/>
       <c r="K9">
         <f>SUM(K11:K21)</f>
-        <v>-3177.16</v>
+        <v>-6257.23</v>
       </c>
       <c r="N9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44766</v>
+        <v>44772</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>1050</v>
@@ -5893,7 +5932,7 @@
       <c r="G12">
         <v>29.72</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="42">
         <v>33.94</v>
       </c>
       <c r="I12" s="29">
@@ -5917,23 +5956,23 @@
         <v>44848</v>
       </c>
       <c r="O12" s="40">
-        <f t="shared" ref="O12:O14" ca="1" si="2">$N$9-N12</f>
-        <v>-82</v>
+        <f t="shared" ref="O12:O17" ca="1" si="2">$N$9-N12</f>
+        <v>-76</v>
       </c>
       <c r="P12" s="29">
         <v>0.56000000000000005</v>
       </c>
-      <c r="Q12" s="29">
-        <f t="shared" ref="Q12" si="3">N12-B12</f>
-        <v>82</v>
+      <c r="Q12" s="40">
+        <f ca="1">N12-TODAY()</f>
+        <v>76</v>
       </c>
       <c r="R12" s="29">
-        <f t="shared" ref="R12" si="4">(1+P12)^(1/Q12)-1</f>
-        <v>5.4377288897551335E-3</v>
+        <f t="shared" ref="R12" ca="1" si="3">(1+P12)^(1/Q12)-1</f>
+        <v>5.8682805188983167E-3</v>
       </c>
       <c r="S12" s="29">
-        <f t="shared" ref="S12" si="5">(1+R12)^92</f>
-        <v>1.6469346948930705</v>
+        <f t="shared" ref="S12" ca="1" si="4">(1+R12)^92</f>
+        <v>1.713098790793659</v>
       </c>
       <c r="T12">
         <f>C3-I12</f>
@@ -5971,14 +6010,14 @@
         <v>28.094557624094499</v>
       </c>
       <c r="I13" s="29">
-        <f t="shared" ref="I13:I14" si="6">G13*E13</f>
+        <f t="shared" ref="I13:I16" si="5">G13*E13</f>
         <v>1129.8</v>
       </c>
       <c r="J13" s="29">
         <v>-1</v>
       </c>
       <c r="K13" s="29">
-        <f t="shared" ref="K13" si="7">J13*I13</f>
+        <f t="shared" ref="K13" si="6">J13*I13</f>
         <v>-1129.8</v>
       </c>
       <c r="L13" s="17" t="s">
@@ -5992,22 +6031,22 @@
       </c>
       <c r="O13" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-82</v>
+        <v>-76</v>
       </c>
       <c r="P13">
         <v>0.18</v>
       </c>
-      <c r="Q13" s="29">
-        <f t="shared" ref="Q13" si="8">N13-B13</f>
-        <v>82</v>
+      <c r="Q13" s="40">
+        <f t="shared" ref="Q13:Q17" ca="1" si="7">N13-TODAY()</f>
+        <v>76</v>
       </c>
       <c r="R13" s="29">
-        <f t="shared" ref="R13" si="9">(1+P13)^(1/Q13)-1</f>
-        <v>2.0205072412979863E-3</v>
+        <f t="shared" ref="R13" ca="1" si="8">(1+P13)^(1/Q13)-1</f>
+        <v>2.1801947347583894E-3</v>
       </c>
       <c r="S13" s="29">
-        <f t="shared" ref="S13:S14" si="10">(1+R13)^92</f>
-        <v>1.2040599356607984</v>
+        <f t="shared" ref="S13:S14" ca="1" si="9">(1+R13)^92</f>
+        <v>1.2218420333147022</v>
       </c>
       <c r="T13" s="39">
         <f>T12-I13</f>
@@ -6045,14 +6084,14 @@
         <v>67.019979399593396</v>
       </c>
       <c r="I14" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1007.16</v>
       </c>
       <c r="J14" s="29">
         <v>-1</v>
       </c>
       <c r="K14" s="29">
-        <f t="shared" ref="K14" si="11">J14*I14</f>
+        <f t="shared" ref="K14:K16" si="10">J14*I14</f>
         <v>-1007.16</v>
       </c>
       <c r="L14" s="39" t="s">
@@ -6066,22 +6105,22 @@
       </c>
       <c r="O14" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-26</v>
+        <v>-20</v>
       </c>
       <c r="P14">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="Q14" s="29">
-        <f t="shared" ref="Q14" si="12">N14-B14</f>
-        <v>26</v>
+      <c r="Q14" s="40">
+        <f t="shared" ca="1" si="7"/>
+        <v>20</v>
       </c>
       <c r="R14" s="29">
-        <f t="shared" ref="R14" si="13">(1+P14)^(1/Q14)-1</f>
-        <v>3.4966515058603154E-3</v>
+        <f t="shared" ref="R14" ca="1" si="11">(1+P14)^(1/Q14)-1</f>
+        <v>4.5480291967769926E-3</v>
       </c>
       <c r="S14" s="29">
-        <f t="shared" si="10"/>
-        <v>1.378685934129833</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.5181159675788036</v>
       </c>
       <c r="T14" s="39">
         <f>T13-I14</f>
@@ -6096,42 +6135,237 @@
       </c>
     </row>
     <row r="15" spans="1:22">
-      <c r="B15" s="1"/>
-      <c r="J15" s="18"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="27"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
+      <c r="A15" s="1">
+        <v>44771</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44772</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15" s="41" cm="1">
+        <f t="array" ref="F15">SUMPRODUCT(($C$11:$C$23=C15)*($E$11:$E$23))</f>
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>116.73</v>
+      </c>
+      <c r="H15" s="38">
+        <v>109.24</v>
+      </c>
+      <c r="I15" s="29">
+        <f t="shared" si="5"/>
+        <v>1050.57</v>
+      </c>
+      <c r="J15" s="29">
+        <v>-1</v>
+      </c>
+      <c r="K15" s="29">
+        <f t="shared" si="10"/>
+        <v>-1050.57</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>1130</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="N15" s="1">
+        <v>44792</v>
+      </c>
+      <c r="O15" s="40">
+        <f t="shared" ca="1" si="2"/>
+        <v>-20</v>
+      </c>
+      <c r="P15" s="41">
+        <v>0.04</v>
+      </c>
+      <c r="Q15" s="40">
+        <f t="shared" ca="1" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="R15" s="29">
+        <f t="shared" ref="R15" ca="1" si="12">(1+P15)^(1/Q15)-1</f>
+        <v>1.9629597456187753E-3</v>
+      </c>
+      <c r="S15" s="29">
+        <f t="shared" ref="S15" ca="1" si="13">(1+R15)^92</f>
+        <v>1.1977146474021529</v>
+      </c>
+      <c r="T15" s="41">
+        <f>T14-I15</f>
+        <v>5772.2699999999995</v>
+      </c>
+      <c r="U15" s="41">
+        <v>6981</v>
+      </c>
+      <c r="V15" s="41">
+        <f>(I15*(1+P15)-I15)</f>
+        <v>42.022799999999961</v>
+      </c>
     </row>
     <row r="16" spans="1:22">
-      <c r="B16" s="1"/>
-      <c r="D16" s="17"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-    </row>
-    <row r="17" spans="2:21">
-      <c r="B17" s="1"/>
-      <c r="J17" s="18"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="27"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-    </row>
-    <row r="18" spans="2:21">
+      <c r="A16" s="1">
+        <v>44771</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44772</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>45</v>
+      </c>
+      <c r="F16" s="18" cm="1">
+        <f t="array" ref="F16">SUMPRODUCT(($C$11:$C$23=C16)*($E$11:$E$23))</f>
+        <v>45</v>
+      </c>
+      <c r="G16">
+        <v>22.62</v>
+      </c>
+      <c r="H16" s="38">
+        <v>19.75487</v>
+      </c>
+      <c r="I16" s="29">
+        <f t="shared" si="5"/>
+        <v>1017.9000000000001</v>
+      </c>
+      <c r="J16" s="29">
+        <v>-1</v>
+      </c>
+      <c r="K16" s="29">
+        <f t="shared" si="10"/>
+        <v>-1017.9000000000001</v>
+      </c>
+      <c r="L16" s="41" t="s">
+        <v>1130</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="N16" s="1">
+        <v>44855</v>
+      </c>
+      <c r="O16" s="40">
+        <f t="shared" ca="1" si="2"/>
+        <v>-83</v>
+      </c>
+      <c r="P16" s="17">
+        <v>0.128</v>
+      </c>
+      <c r="Q16" s="40">
+        <f t="shared" ca="1" si="7"/>
+        <v>83</v>
+      </c>
+      <c r="R16" s="29">
+        <f t="shared" ref="R16" ca="1" si="14">(1+P16)^(1/Q16)-1</f>
+        <v>1.4522119107551745E-3</v>
+      </c>
+      <c r="S16" s="29">
+        <f t="shared" ref="S16" ca="1" si="15">(1+R16)^92</f>
+        <v>1.142828785138678</v>
+      </c>
+      <c r="T16" s="41">
+        <f>T15-I16</f>
+        <v>4754.369999999999</v>
+      </c>
+      <c r="U16" s="41">
+        <v>6981</v>
+      </c>
+      <c r="V16">
+        <f>(I16*(1+P16)-I16)</f>
+        <v>130.29120000000012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="1">
+        <v>44771</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44772</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="41">
+        <v>45</v>
+      </c>
+      <c r="F17" s="18" cm="1">
+        <f t="array" ref="F17">SUMPRODUCT(($C$11:$C$23=C17)*($E$11:$E$23))</f>
+        <v>45</v>
+      </c>
+      <c r="G17">
+        <v>22.48</v>
+      </c>
+      <c r="H17" s="41">
+        <v>19.75487</v>
+      </c>
+      <c r="I17" s="29">
+        <f t="shared" ref="I17" si="16">G17*E17</f>
+        <v>1011.6</v>
+      </c>
+      <c r="J17" s="29">
+        <v>-1</v>
+      </c>
+      <c r="K17" s="29">
+        <f t="shared" ref="K17" si="17">J17*I17</f>
+        <v>-1011.6</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>1136</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>1135</v>
+      </c>
+      <c r="N17" s="1">
+        <v>44848</v>
+      </c>
+      <c r="O17" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>-76</v>
+      </c>
+      <c r="P17" s="41">
+        <v>0.128</v>
+      </c>
+      <c r="Q17" s="40">
+        <f t="shared" ca="1" si="7"/>
+        <v>76</v>
+      </c>
+      <c r="R17" s="29">
+        <f t="shared" ref="R17" ca="1" si="18">(1+P17)^(1/Q17)-1</f>
+        <v>1.5860742910454029E-3</v>
+      </c>
+      <c r="S17" s="29">
+        <f t="shared" ref="S17" ca="1" si="19">(1+R17)^92</f>
+        <v>1.1569685181371452</v>
+      </c>
+      <c r="T17" s="41">
+        <f>T16-I17</f>
+        <v>3742.7699999999991</v>
+      </c>
+      <c r="U17" s="41">
+        <v>6981</v>
+      </c>
+      <c r="V17" s="41">
+        <f>(I17*(1+P17)-I17)</f>
+        <v>129.48480000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="B18" s="1"/>
       <c r="D18" s="17"/>
       <c r="J18" s="18"/>
@@ -6144,7 +6378,7 @@
       <c r="R18" s="17"/>
       <c r="S18" s="17"/>
     </row>
-    <row r="19" spans="2:21">
+    <row r="19" spans="1:22">
       <c r="B19" s="1"/>
       <c r="D19" s="17"/>
       <c r="J19" s="18"/>
@@ -6158,7 +6392,7 @@
       <c r="R19" s="17"/>
       <c r="S19" s="17"/>
     </row>
-    <row r="20" spans="2:21">
+    <row r="20" spans="1:22">
       <c r="B20" s="1"/>
       <c r="D20" s="17"/>
       <c r="J20" s="18"/>
@@ -6172,7 +6406,7 @@
       <c r="R20" s="17"/>
       <c r="S20" s="17"/>
     </row>
-    <row r="21" spans="2:21">
+    <row r="21" spans="1:22">
       <c r="B21" s="1"/>
       <c r="D21" s="17"/>
       <c r="J21" s="18"/>
@@ -6185,7 +6419,7 @@
       <c r="R21" s="17"/>
       <c r="S21" s="17"/>
     </row>
-    <row r="22" spans="2:21">
+    <row r="22" spans="1:22">
       <c r="B22" s="1"/>
       <c r="J22" s="18"/>
       <c r="L22" s="17"/>
@@ -6196,7 +6430,7 @@
       <c r="R22" s="17"/>
       <c r="S22" s="17"/>
     </row>
-    <row r="23" spans="2:21">
+    <row r="23" spans="1:22">
       <c r="B23" s="1"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -6212,7 +6446,7 @@
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
     </row>
-    <row r="24" spans="2:21">
+    <row r="24" spans="1:22">
       <c r="B24" s="1"/>
       <c r="E24" s="18"/>
       <c r="F24" s="26"/>
@@ -6226,7 +6460,7 @@
       <c r="R24" s="26"/>
       <c r="S24" s="26"/>
     </row>
-    <row r="25" spans="2:21">
+    <row r="25" spans="1:22">
       <c r="B25" s="1"/>
       <c r="D25" s="26"/>
       <c r="F25" s="26"/>
@@ -6240,7 +6474,7 @@
       <c r="R25" s="26"/>
       <c r="S25" s="26"/>
     </row>
-    <row r="26" spans="2:21">
+    <row r="26" spans="1:22">
       <c r="B26" s="1"/>
       <c r="C26" s="26"/>
       <c r="F26" s="26"/>
@@ -6253,7 +6487,7 @@
       <c r="R26" s="26"/>
       <c r="S26" s="26"/>
     </row>
-    <row r="27" spans="2:21">
+    <row r="27" spans="1:22">
       <c r="B27" s="1"/>
       <c r="D27" s="26"/>
       <c r="F27" s="26"/>
@@ -6267,7 +6501,7 @@
       <c r="R27" s="26"/>
       <c r="S27" s="26"/>
     </row>
-    <row r="28" spans="2:21">
+    <row r="28" spans="1:22">
       <c r="B28" s="1"/>
       <c r="D28" s="26"/>
       <c r="J28" s="26"/>
@@ -6279,7 +6513,7 @@
       <c r="R28" s="26"/>
       <c r="S28" s="26"/>
     </row>
-    <row r="29" spans="2:21">
+    <row r="29" spans="1:22">
       <c r="B29" s="1"/>
       <c r="D29" s="26"/>
       <c r="J29" s="26"/>
@@ -6292,7 +6526,7 @@
       <c r="R29" s="26"/>
       <c r="S29" s="26"/>
     </row>
-    <row r="30" spans="2:21">
+    <row r="30" spans="1:22">
       <c r="B30" s="1"/>
       <c r="J30" s="31"/>
       <c r="K30" s="31"/>
@@ -6302,7 +6536,7 @@
       <c r="R30" s="31"/>
       <c r="S30" s="31"/>
     </row>
-    <row r="31" spans="2:21">
+    <row r="31" spans="1:22">
       <c r="B31" s="1"/>
       <c r="J31" s="30"/>
       <c r="K31" s="30"/>
@@ -6311,7 +6545,7 @@
       <c r="T31" s="36"/>
       <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="2:21">
+    <row r="32" spans="1:22">
       <c r="B32" s="1"/>
       <c r="J32" s="31"/>
       <c r="K32" s="31"/>
@@ -6647,10 +6881,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="42"/>
+      <c r="B35" s="44"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -6707,10 +6941,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="42"/>
+      <c r="B44" s="44"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -7196,10 +7430,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="42"/>
+      <c r="B38" s="44"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -7256,10 +7490,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="42"/>
+      <c r="B47" s="44"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>
@@ -8642,10 +8876,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="42"/>
+      <c r="B38" s="44"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -8702,10 +8936,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="42"/>
+      <c r="B47" s="44"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -9028,10 +9262,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="42"/>
+      <c r="B35" s="44"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -9088,10 +9322,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="42"/>
+      <c r="B44" s="44"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -9588,10 +9822,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="42"/>
+      <c r="B15" s="44"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -9648,10 +9882,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="42"/>
+      <c r="B24" s="44"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -9966,10 +10200,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="42"/>
+      <c r="B32" s="44"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -10026,10 +10260,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="42"/>
+      <c r="B41" s="44"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -13760,10 +13994,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="42"/>
+      <c r="B35" s="44"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -13820,10 +14054,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="42"/>
+      <c r="B44" s="44"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -14151,10 +14385,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="42"/>
+      <c r="B35" s="44"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -14211,10 +14445,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="42"/>
+      <c r="B44" s="44"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -15354,10 +15588,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="42"/>
+      <c r="B35" s="44"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -15414,10 +15648,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="42"/>
+      <c r="B44" s="44"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -16030,10 +16264,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="41" t="s">
+      <c r="A63" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="42"/>
+      <c r="B63" s="44"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -16090,10 +16324,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="41" t="s">
+      <c r="A72" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="42"/>
+      <c r="B72" s="44"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -16553,10 +16787,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="42"/>
+      <c r="B32" s="44"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -16613,10 +16847,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="42"/>
+      <c r="B41" s="44"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -17704,10 +17938,10 @@
       <c r="A31" s="21"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="42"/>
+      <c r="B32" s="44"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -17764,10 +17998,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="42"/>
+      <c r="B41" s="44"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>

</xml_diff>

<commit_message>
added CNN LSTM bidirectional attention
</commit_message>
<xml_diff>
--- a/code/Screener/data/interim/record.xlsx
+++ b/code/Screener/data/interim/record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\data\interim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFD1AF3-BDEE-40D2-B034-279556C81F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B8A4B7-BF36-473C-B17E-AC8C05A74768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="-10770" windowWidth="20730" windowHeight="11835" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
   <sheets>
     <sheet name="Record book" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1146">
   <si>
     <t>MCK</t>
   </si>
@@ -3483,6 +3483,33 @@
   </si>
   <si>
     <t>Industrial</t>
+  </si>
+  <si>
+    <t>Days until Sell</t>
+  </si>
+  <si>
+    <t>CNP</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>Sell date</t>
+  </si>
+  <si>
+    <t>Stop Loss Price</t>
+  </si>
+  <si>
+    <t>Buy Price</t>
+  </si>
+  <si>
+    <t>Sheet/Order Date</t>
   </si>
 </sst>
 </file>
@@ -3597,7 +3624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3685,6 +3712,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5775,7 +5803,7 @@
   <dimension ref="A3:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5797,6 +5825,9 @@
       <c r="C3">
         <v>10000</v>
       </c>
+      <c r="G3" t="s">
+        <v>1141</v>
+      </c>
     </row>
     <row r="4" spans="1:22">
       <c r="B4" t="s">
@@ -5807,28 +5838,47 @@
       </c>
       <c r="E4" s="1">
         <f ca="1">TODAY()</f>
-        <v>44772</v>
+        <v>44787</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="G6" t="s">
+        <v>1143</v>
       </c>
     </row>
     <row r="7" spans="1:22">
       <c r="D7" t="s">
         <v>1132</v>
       </c>
+      <c r="G7" t="s">
+        <v>1144</v>
+      </c>
     </row>
     <row r="8" spans="1:22">
       <c r="D8" t="s">
         <v>1133</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1145</v>
       </c>
     </row>
     <row r="9" spans="1:22">
       <c r="I9" s="18"/>
       <c r="K9">
         <f>SUM(K11:K21)</f>
-        <v>-6257.23</v>
+        <v>-6817.93</v>
       </c>
       <c r="N9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44772</v>
+        <v>44787</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>1050</v>
@@ -5884,6 +5934,9 @@
       <c r="O10" s="15"/>
       <c r="P10" s="15" t="s">
         <v>110</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>1137</v>
       </c>
       <c r="R10" s="15" t="s">
         <v>413</v>
@@ -5956,30 +6009,30 @@
         <v>44848</v>
       </c>
       <c r="O12" s="40">
-        <f t="shared" ref="O12:O17" ca="1" si="2">$N$9-N12</f>
-        <v>-76</v>
+        <f t="shared" ref="O12:O19" ca="1" si="2">$N$9-N12</f>
+        <v>-61</v>
       </c>
       <c r="P12" s="29">
         <v>0.56000000000000005</v>
       </c>
       <c r="Q12" s="40">
         <f ca="1">N12-TODAY()</f>
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="R12" s="29">
         <f t="shared" ref="R12" ca="1" si="3">(1+P12)^(1/Q12)-1</f>
-        <v>5.8682805188983167E-3</v>
+        <v>7.3165677328057566E-3</v>
       </c>
       <c r="S12" s="29">
         <f t="shared" ref="S12" ca="1" si="4">(1+R12)^92</f>
-        <v>1.713098790793659</v>
+        <v>1.9555543292902902</v>
       </c>
       <c r="T12">
         <f>C3-I12</f>
         <v>8959.7999999999993</v>
       </c>
       <c r="V12">
-        <f>(I12*(1+P12)-I12)</f>
+        <f t="shared" ref="V12:V19" si="5">(I12*(1+P12)-I12)</f>
         <v>582.51200000000017</v>
       </c>
     </row>
@@ -6010,14 +6063,14 @@
         <v>28.094557624094499</v>
       </c>
       <c r="I13" s="29">
-        <f t="shared" ref="I13:I16" si="5">G13*E13</f>
+        <f t="shared" ref="I13:I16" si="6">G13*E13</f>
         <v>1129.8</v>
       </c>
       <c r="J13" s="29">
         <v>-1</v>
       </c>
       <c r="K13" s="29">
-        <f t="shared" ref="K13" si="6">J13*I13</f>
+        <f t="shared" ref="K13" si="7">J13*I13</f>
         <v>-1129.8</v>
       </c>
       <c r="L13" s="17" t="s">
@@ -6031,29 +6084,29 @@
       </c>
       <c r="O13" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-76</v>
+        <v>-61</v>
       </c>
       <c r="P13">
         <v>0.18</v>
       </c>
       <c r="Q13" s="40">
-        <f t="shared" ref="Q13:Q17" ca="1" si="7">N13-TODAY()</f>
-        <v>76</v>
+        <f t="shared" ref="Q13:Q19" ca="1" si="8">N13-TODAY()</f>
+        <v>61</v>
       </c>
       <c r="R13" s="29">
-        <f t="shared" ref="R13" ca="1" si="8">(1+P13)^(1/Q13)-1</f>
-        <v>2.1801947347583894E-3</v>
+        <f t="shared" ref="R13" ca="1" si="9">(1+P13)^(1/Q13)-1</f>
+        <v>2.7170359201655891E-3</v>
       </c>
       <c r="S13" s="29">
-        <f t="shared" ref="S13:S14" ca="1" si="9">(1+R13)^92</f>
-        <v>1.2218420333147022</v>
+        <f t="shared" ref="S13:S14" ca="1" si="10">(1+R13)^92</f>
+        <v>1.2835482760543</v>
       </c>
       <c r="T13" s="39">
         <f>T12-I13</f>
         <v>7829.9999999999991</v>
       </c>
       <c r="V13" s="39">
-        <f>(I13*(1+P13)-I13)</f>
+        <f t="shared" si="5"/>
         <v>203.36400000000003</v>
       </c>
     </row>
@@ -6084,14 +6137,14 @@
         <v>67.019979399593396</v>
       </c>
       <c r="I14" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1007.16</v>
       </c>
       <c r="J14" s="29">
         <v>-1</v>
       </c>
       <c r="K14" s="29">
-        <f t="shared" ref="K14:K16" si="10">J14*I14</f>
+        <f t="shared" ref="K14:K16" si="11">J14*I14</f>
         <v>-1007.16</v>
       </c>
       <c r="L14" s="39" t="s">
@@ -6105,22 +6158,22 @@
       </c>
       <c r="O14" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-20</v>
+        <v>-5</v>
       </c>
       <c r="P14">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="Q14" s="40">
-        <f t="shared" ca="1" si="7"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>5</v>
       </c>
       <c r="R14" s="29">
-        <f t="shared" ref="R14" ca="1" si="11">(1+P14)^(1/Q14)-1</f>
-        <v>4.5480291967769926E-3</v>
+        <f t="shared" ref="R14" ca="1" si="12">(1+P14)^(1/Q14)-1</f>
+        <v>1.8316600928512949E-2</v>
       </c>
       <c r="S14" s="29">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.5181159675788036</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>5.3115318845086508</v>
       </c>
       <c r="T14" s="39">
         <f>T13-I14</f>
@@ -6130,7 +6183,7 @@
         <v>6981</v>
       </c>
       <c r="V14" s="39">
-        <f>(I14*(1+P14)-I14)</f>
+        <f t="shared" si="5"/>
         <v>95.6801999999999</v>
       </c>
     </row>
@@ -6161,14 +6214,14 @@
         <v>109.24</v>
       </c>
       <c r="I15" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1050.57</v>
       </c>
       <c r="J15" s="29">
         <v>-1</v>
       </c>
       <c r="K15" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1050.57</v>
       </c>
       <c r="L15" s="17" t="s">
@@ -6182,22 +6235,22 @@
       </c>
       <c r="O15" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-20</v>
+        <v>-5</v>
       </c>
       <c r="P15" s="41">
         <v>0.04</v>
       </c>
       <c r="Q15" s="40">
-        <f t="shared" ca="1" si="7"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>5</v>
       </c>
       <c r="R15" s="29">
-        <f t="shared" ref="R15" ca="1" si="12">(1+P15)^(1/Q15)-1</f>
-        <v>1.9629597456187753E-3</v>
+        <f t="shared" ref="R15" ca="1" si="13">(1+P15)^(1/Q15)-1</f>
+        <v>7.8749885178921453E-3</v>
       </c>
       <c r="S15" s="29">
-        <f t="shared" ref="S15" ca="1" si="13">(1+R15)^92</f>
-        <v>1.1977146474021529</v>
+        <f t="shared" ref="S15" ca="1" si="14">(1+R15)^92</f>
+        <v>2.0578487108854202</v>
       </c>
       <c r="T15" s="41">
         <f>T14-I15</f>
@@ -6207,7 +6260,7 @@
         <v>6981</v>
       </c>
       <c r="V15" s="41">
-        <f>(I15*(1+P15)-I15)</f>
+        <f t="shared" si="5"/>
         <v>42.022799999999961</v>
       </c>
     </row>
@@ -6238,14 +6291,14 @@
         <v>19.75487</v>
       </c>
       <c r="I16" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1017.9000000000001</v>
       </c>
       <c r="J16" s="29">
         <v>-1</v>
       </c>
       <c r="K16" s="29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-1017.9000000000001</v>
       </c>
       <c r="L16" s="41" t="s">
@@ -6259,22 +6312,22 @@
       </c>
       <c r="O16" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-83</v>
+        <v>-68</v>
       </c>
       <c r="P16" s="17">
         <v>0.128</v>
       </c>
       <c r="Q16" s="40">
-        <f t="shared" ca="1" si="7"/>
-        <v>83</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>68</v>
       </c>
       <c r="R16" s="29">
-        <f t="shared" ref="R16" ca="1" si="14">(1+P16)^(1/Q16)-1</f>
-        <v>1.4522119107551745E-3</v>
+        <f t="shared" ref="R16" ca="1" si="15">(1+P16)^(1/Q16)-1</f>
+        <v>1.7728365769162924E-3</v>
       </c>
       <c r="S16" s="29">
-        <f t="shared" ref="S16" ca="1" si="15">(1+R16)^92</f>
-        <v>1.142828785138678</v>
+        <f t="shared" ref="S16" ca="1" si="16">(1+R16)^92</f>
+        <v>1.1769855603767694</v>
       </c>
       <c r="T16" s="41">
         <f>T15-I16</f>
@@ -6284,7 +6337,7 @@
         <v>6981</v>
       </c>
       <c r="V16">
-        <f>(I16*(1+P16)-I16)</f>
+        <f t="shared" si="5"/>
         <v>130.29120000000012</v>
       </c>
     </row>
@@ -6315,14 +6368,14 @@
         <v>19.75487</v>
       </c>
       <c r="I17" s="29">
-        <f t="shared" ref="I17" si="16">G17*E17</f>
+        <f t="shared" ref="I17:I19" si="17">G17*E17</f>
         <v>1011.6</v>
       </c>
       <c r="J17" s="29">
         <v>-1</v>
       </c>
       <c r="K17" s="29">
-        <f t="shared" ref="K17" si="17">J17*I17</f>
+        <f t="shared" ref="K17" si="18">J17*I17</f>
         <v>-1011.6</v>
       </c>
       <c r="L17" s="17" t="s">
@@ -6336,22 +6389,22 @@
       </c>
       <c r="O17" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>-76</v>
+        <v>-61</v>
       </c>
       <c r="P17" s="41">
         <v>0.128</v>
       </c>
       <c r="Q17" s="40">
-        <f t="shared" ca="1" si="7"/>
-        <v>76</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>61</v>
       </c>
       <c r="R17" s="29">
-        <f t="shared" ref="R17" ca="1" si="18">(1+P17)^(1/Q17)-1</f>
-        <v>1.5860742910454029E-3</v>
+        <f t="shared" ref="R17:R19" ca="1" si="19">(1+P17)^(1/Q17)-1</f>
+        <v>1.9764777619051266E-3</v>
       </c>
       <c r="S17" s="29">
-        <f t="shared" ref="S17" ca="1" si="19">(1+R17)^92</f>
-        <v>1.1569685181371452</v>
+        <f t="shared" ref="S17:S19" ca="1" si="20">(1+R17)^92</f>
+        <v>1.1992021889705322</v>
       </c>
       <c r="T17" s="41">
         <f>T16-I17</f>
@@ -6361,36 +6414,163 @@
         <v>6981</v>
       </c>
       <c r="V17" s="41">
-        <f>(I17*(1+P17)-I17)</f>
+        <f t="shared" si="5"/>
         <v>129.48480000000006</v>
       </c>
     </row>
     <row r="18" spans="1:22">
-      <c r="B18" s="1"/>
-      <c r="D18" s="17"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="27"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
+      <c r="A18" s="1">
+        <v>44785</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44787</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18" s="18" cm="1">
+        <f t="array" ref="F18">SUMPRODUCT(($C$11:$C$23=C18)*($E$11:$E$23))</f>
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="H18" s="38">
+        <v>30.15</v>
+      </c>
+      <c r="I18" s="29">
+        <f t="shared" si="17"/>
+        <v>261.60000000000002</v>
+      </c>
+      <c r="J18" s="29">
+        <v>-1</v>
+      </c>
+      <c r="K18" s="29">
+        <f t="shared" ref="K18" si="21">J18*I18</f>
+        <v>-261.60000000000002</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>1140</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="N18" s="1">
+        <v>44869</v>
+      </c>
+      <c r="O18" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>-82</v>
+      </c>
+      <c r="P18">
+        <v>0.113</v>
+      </c>
+      <c r="Q18" s="40">
+        <f t="shared" ca="1" si="8"/>
+        <v>82</v>
+      </c>
+      <c r="R18" s="29">
+        <f t="shared" ca="1" si="19"/>
+        <v>1.3064511072879981E-3</v>
+      </c>
+      <c r="S18" s="29">
+        <f t="shared" ca="1" si="20"/>
+        <v>1.1276265851314986</v>
+      </c>
+      <c r="T18" s="43">
+        <f>T17-I18</f>
+        <v>3481.1699999999992</v>
+      </c>
+      <c r="U18" s="43">
+        <v>6981</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="5"/>
+        <v>29.560799999999972</v>
+      </c>
     </row>
     <row r="19" spans="1:22">
-      <c r="B19" s="1"/>
-      <c r="D19" s="17"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
+      <c r="A19" s="1">
+        <v>44785</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44787</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" s="18" cm="1">
+        <f t="array" ref="F19">SUMPRODUCT(($C$11:$C$23=C19)*($E$11:$E$23))</f>
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>99.7</v>
+      </c>
+      <c r="H19" s="38">
+        <v>99.7</v>
+      </c>
+      <c r="I19" s="29">
+        <f t="shared" si="17"/>
+        <v>299.10000000000002</v>
+      </c>
+      <c r="J19" s="29">
+        <v>-1</v>
+      </c>
+      <c r="K19" s="29">
+        <f t="shared" ref="K19" si="22">J19*I19</f>
+        <v>-299.10000000000002</v>
+      </c>
+      <c r="L19" s="43" t="s">
+        <v>1140</v>
+      </c>
+      <c r="M19" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="N19" s="1">
+        <v>44862</v>
+      </c>
+      <c r="O19" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>-75</v>
+      </c>
+      <c r="P19" s="17">
+        <v>0.08</v>
+      </c>
+      <c r="Q19" s="40">
+        <f t="shared" ca="1" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="R19" s="29">
+        <f t="shared" ca="1" si="19"/>
+        <v>1.0266738843331957E-3</v>
+      </c>
+      <c r="S19" s="29">
+        <f t="shared" ca="1" si="20"/>
+        <v>1.0990053503540307</v>
+      </c>
+      <c r="T19" s="43">
+        <f>T18-I19</f>
+        <v>3182.0699999999993</v>
+      </c>
+      <c r="U19" s="43">
+        <v>6981</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="5"/>
+        <v>23.927999999999997</v>
+      </c>
     </row>
     <row r="20" spans="1:22">
       <c r="B20" s="1"/>
@@ -6881,10 +7061,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="44"/>
+      <c r="B35" s="45"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -6941,10 +7121,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="44"/>
+      <c r="B44" s="45"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -7430,10 +7610,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="44"/>
+      <c r="B38" s="45"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -7490,10 +7670,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="44"/>
+      <c r="B47" s="45"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>
@@ -8876,10 +9056,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="44"/>
+      <c r="B38" s="45"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -8936,10 +9116,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="44"/>
+      <c r="B47" s="45"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -9262,10 +9442,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="44"/>
+      <c r="B35" s="45"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -9322,10 +9502,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="44"/>
+      <c r="B44" s="45"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -9822,10 +10002,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="44"/>
+      <c r="B15" s="45"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -9882,10 +10062,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="44"/>
+      <c r="B24" s="45"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -10200,10 +10380,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="44"/>
+      <c r="B32" s="45"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -10260,10 +10440,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="44"/>
+      <c r="B41" s="45"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -13994,10 +14174,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="44"/>
+      <c r="B35" s="45"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -14054,10 +14234,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="44"/>
+      <c r="B44" s="45"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -14385,10 +14565,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="44"/>
+      <c r="B35" s="45"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -14445,10 +14625,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="44"/>
+      <c r="B44" s="45"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -15588,10 +15768,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="44"/>
+      <c r="B35" s="45"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -15648,10 +15828,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="44"/>
+      <c r="B44" s="45"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -16264,10 +16444,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="44"/>
+      <c r="B63" s="45"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -16324,10 +16504,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="43" t="s">
+      <c r="A72" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="44"/>
+      <c r="B72" s="45"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -16787,10 +16967,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="44"/>
+      <c r="B32" s="45"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -16847,10 +17027,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="44"/>
+      <c r="B41" s="45"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -17938,10 +18118,10 @@
       <c r="A31" s="21"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="44"/>
+      <c r="B32" s="45"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -17998,10 +18178,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="44"/>
+      <c r="B41" s="45"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>

</xml_diff>

<commit_message>
mxn peso to usd
</commit_message>
<xml_diff>
--- a/code/Screener/data/interim/record.xlsx
+++ b/code/Screener/data/interim/record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\data\interim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B8A4B7-BF36-473C-B17E-AC8C05A74768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF43118-C03B-4E13-A526-ECFC04D80328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1147">
   <si>
     <t>MCK</t>
   </si>
@@ -3510,6 +3510,9 @@
   </si>
   <si>
     <t>Sheet/Order Date</t>
+  </si>
+  <si>
+    <t>Sell</t>
   </si>
 </sst>
 </file>
@@ -3624,7 +3627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3712,6 +3715,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5803,7 +5807,7 @@
   <dimension ref="A3:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5838,7 +5842,7 @@
       </c>
       <c r="E4" s="1">
         <f ca="1">TODAY()</f>
-        <v>44787</v>
+        <v>44792</v>
       </c>
       <c r="G4" t="s">
         <v>1142</v>
@@ -5874,11 +5878,11 @@
       <c r="I9" s="18"/>
       <c r="K9">
         <f>SUM(K11:K21)</f>
-        <v>-6817.93</v>
+        <v>-4492.01</v>
       </c>
       <c r="N9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44787</v>
+        <v>44792</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>1050</v>
@@ -5980,19 +5984,18 @@
       </c>
       <c r="F12" s="39" cm="1">
         <f t="array" ref="F12">SUMPRODUCT(($C$11:$C$23=C12)*($E$11:$E$23))</f>
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="G12">
         <v>29.72</v>
       </c>
-      <c r="H12" s="42">
-        <v>33.94</v>
-      </c>
+      <c r="H12" s="42"/>
       <c r="I12" s="29">
         <f t="shared" ref="I12" si="0">G12*E12</f>
         <v>1040.2</v>
       </c>
       <c r="J12" s="29">
+        <f>IF(D12="BUY",-1,1)</f>
         <v>-1</v>
       </c>
       <c r="K12" s="29">
@@ -6010,22 +6013,22 @@
       </c>
       <c r="O12" s="40">
         <f t="shared" ref="O12:O19" ca="1" si="2">$N$9-N12</f>
-        <v>-61</v>
+        <v>-56</v>
       </c>
       <c r="P12" s="29">
         <v>0.56000000000000005</v>
       </c>
       <c r="Q12" s="40">
         <f ca="1">N12-TODAY()</f>
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="R12" s="29">
         <f t="shared" ref="R12" ca="1" si="3">(1+P12)^(1/Q12)-1</f>
-        <v>7.3165677328057566E-3</v>
+        <v>7.9724301533745656E-3</v>
       </c>
       <c r="S12" s="29">
         <f t="shared" ref="S12" ca="1" si="4">(1+R12)^92</f>
-        <v>1.9555543292902902</v>
+        <v>2.0762331738086672</v>
       </c>
       <c r="T12">
         <f>C3-I12</f>
@@ -6067,10 +6070,11 @@
         <v>1129.8</v>
       </c>
       <c r="J13" s="29">
+        <f t="shared" ref="J13:J21" si="7">IF(D13="BUY",-1,1)</f>
         <v>-1</v>
       </c>
       <c r="K13" s="29">
-        <f t="shared" ref="K13" si="7">J13*I13</f>
+        <f t="shared" ref="K13" si="8">J13*I13</f>
         <v>-1129.8</v>
       </c>
       <c r="L13" s="17" t="s">
@@ -6084,25 +6088,25 @@
       </c>
       <c r="O13" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-61</v>
+        <v>-56</v>
       </c>
       <c r="P13">
         <v>0.18</v>
       </c>
       <c r="Q13" s="40">
-        <f t="shared" ref="Q13:Q19" ca="1" si="8">N13-TODAY()</f>
-        <v>61</v>
+        <f t="shared" ref="Q13:Q19" ca="1" si="9">N13-TODAY()</f>
+        <v>56</v>
       </c>
       <c r="R13" s="29">
-        <f t="shared" ref="R13" ca="1" si="9">(1+P13)^(1/Q13)-1</f>
-        <v>2.7170359201655891E-3</v>
+        <f t="shared" ref="R13" ca="1" si="10">(1+P13)^(1/Q13)-1</f>
+        <v>2.95998710913703E-3</v>
       </c>
       <c r="S13" s="29">
-        <f t="shared" ref="S13:S14" ca="1" si="10">(1+R13)^92</f>
-        <v>1.2835482760543</v>
+        <f t="shared" ref="S13:S14" ca="1" si="11">(1+R13)^92</f>
+        <v>1.3124775065877488</v>
       </c>
       <c r="T13" s="39">
-        <f>T12-I13</f>
+        <f t="shared" ref="T13:T19" si="12">T12-I13</f>
         <v>7829.9999999999991</v>
       </c>
       <c r="V13" s="39">
@@ -6141,10 +6145,11 @@
         <v>1007.16</v>
       </c>
       <c r="J14" s="29">
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="K14" s="29">
-        <f t="shared" ref="K14:K16" si="11">J14*I14</f>
+        <f t="shared" ref="K14:K16" si="13">J14*I14</f>
         <v>-1007.16</v>
       </c>
       <c r="L14" s="39" t="s">
@@ -6158,25 +6163,25 @@
       </c>
       <c r="O14" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="P14">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="Q14" s="40">
-        <f t="shared" ca="1" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="R14" s="29">
-        <f t="shared" ref="R14" ca="1" si="12">(1+P14)^(1/Q14)-1</f>
-        <v>1.8316600928512949E-2</v>
-      </c>
-      <c r="S14" s="29">
-        <f t="shared" ca="1" si="10"/>
-        <v>5.3115318845086508</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="29" t="e">
+        <f t="shared" ref="R14" ca="1" si="14">(1+P14)^(1/Q14)-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S14" s="29" t="e">
+        <f t="shared" ca="1" si="11"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="T14" s="39">
-        <f>T13-I14</f>
+        <f t="shared" si="12"/>
         <v>6822.8399999999992</v>
       </c>
       <c r="U14" s="39">
@@ -6205,7 +6210,7 @@
       </c>
       <c r="F15" s="41" cm="1">
         <f t="array" ref="F15">SUMPRODUCT(($C$11:$C$23=C15)*($E$11:$E$23))</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G15">
         <v>116.73</v>
@@ -6218,10 +6223,11 @@
         <v>1050.57</v>
       </c>
       <c r="J15" s="29">
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="K15" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1050.57</v>
       </c>
       <c r="L15" s="17" t="s">
@@ -6235,25 +6241,25 @@
       </c>
       <c r="O15" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="P15" s="41">
         <v>0.04</v>
       </c>
       <c r="Q15" s="40">
-        <f t="shared" ca="1" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="R15" s="29">
-        <f t="shared" ref="R15" ca="1" si="13">(1+P15)^(1/Q15)-1</f>
-        <v>7.8749885178921453E-3</v>
-      </c>
-      <c r="S15" s="29">
-        <f t="shared" ref="S15" ca="1" si="14">(1+R15)^92</f>
-        <v>2.0578487108854202</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="29" t="e">
+        <f t="shared" ref="R15" ca="1" si="15">(1+P15)^(1/Q15)-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S15" s="29" t="e">
+        <f t="shared" ref="S15" ca="1" si="16">(1+R15)^92</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="T15" s="41">
-        <f>T14-I15</f>
+        <f t="shared" si="12"/>
         <v>5772.2699999999995</v>
       </c>
       <c r="U15" s="41">
@@ -6295,10 +6301,11 @@
         <v>1017.9000000000001</v>
       </c>
       <c r="J16" s="29">
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="K16" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1017.9000000000001</v>
       </c>
       <c r="L16" s="41" t="s">
@@ -6312,25 +6319,25 @@
       </c>
       <c r="O16" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-68</v>
+        <v>-63</v>
       </c>
       <c r="P16" s="17">
         <v>0.128</v>
       </c>
       <c r="Q16" s="40">
-        <f t="shared" ca="1" si="8"/>
-        <v>68</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>63</v>
       </c>
       <c r="R16" s="29">
-        <f t="shared" ref="R16" ca="1" si="15">(1+P16)^(1/Q16)-1</f>
-        <v>1.7728365769162924E-3</v>
+        <f t="shared" ref="R16" ca="1" si="17">(1+P16)^(1/Q16)-1</f>
+        <v>1.9136724380177661E-3</v>
       </c>
       <c r="S16" s="29">
-        <f t="shared" ref="S16" ca="1" si="16">(1+R16)^92</f>
-        <v>1.1769855603767694</v>
+        <f t="shared" ref="S16" ca="1" si="18">(1+R16)^92</f>
+        <v>1.192306445036563</v>
       </c>
       <c r="T16" s="41">
-        <f>T15-I16</f>
+        <f t="shared" si="12"/>
         <v>4754.369999999999</v>
       </c>
       <c r="U16" s="41">
@@ -6368,14 +6375,15 @@
         <v>19.75487</v>
       </c>
       <c r="I17" s="29">
-        <f t="shared" ref="I17:I19" si="17">G17*E17</f>
+        <f t="shared" ref="I17:I21" si="19">G17*E17</f>
         <v>1011.6</v>
       </c>
       <c r="J17" s="29">
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="K17" s="29">
-        <f t="shared" ref="K17" si="18">J17*I17</f>
+        <f t="shared" ref="K17" si="20">J17*I17</f>
         <v>-1011.6</v>
       </c>
       <c r="L17" s="17" t="s">
@@ -6389,25 +6397,25 @@
       </c>
       <c r="O17" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>-61</v>
+        <v>-56</v>
       </c>
       <c r="P17" s="41">
         <v>0.128</v>
       </c>
       <c r="Q17" s="40">
-        <f t="shared" ca="1" si="8"/>
-        <v>61</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>56</v>
       </c>
       <c r="R17" s="29">
-        <f t="shared" ref="R17:R19" ca="1" si="19">(1+P17)^(1/Q17)-1</f>
-        <v>1.9764777619051266E-3</v>
+        <f t="shared" ref="R17:R19" ca="1" si="21">(1+P17)^(1/Q17)-1</f>
+        <v>2.1531388435505061E-3</v>
       </c>
       <c r="S17" s="29">
-        <f t="shared" ref="S17:S19" ca="1" si="20">(1+R17)^92</f>
-        <v>1.1992021889705322</v>
+        <f t="shared" ref="S17:S19" ca="1" si="22">(1+R17)^92</f>
+        <v>1.2188110360169528</v>
       </c>
       <c r="T17" s="41">
-        <f>T16-I17</f>
+        <f t="shared" si="12"/>
         <v>3742.7699999999991</v>
       </c>
       <c r="U17" s="41">
@@ -6445,14 +6453,15 @@
         <v>30.15</v>
       </c>
       <c r="I18" s="29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>261.60000000000002</v>
       </c>
       <c r="J18" s="29">
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="K18" s="29">
-        <f t="shared" ref="K18" si="21">J18*I18</f>
+        <f t="shared" ref="K18" si="23">J18*I18</f>
         <v>-261.60000000000002</v>
       </c>
       <c r="L18" s="17" t="s">
@@ -6466,25 +6475,25 @@
       </c>
       <c r="O18" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>-82</v>
+        <v>-77</v>
       </c>
       <c r="P18">
         <v>0.113</v>
       </c>
       <c r="Q18" s="40">
-        <f t="shared" ca="1" si="8"/>
-        <v>82</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>77</v>
       </c>
       <c r="R18" s="29">
-        <f t="shared" ca="1" si="19"/>
-        <v>1.3064511072879981E-3</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1.3913445852586914E-3</v>
       </c>
       <c r="S18" s="29">
-        <f t="shared" ca="1" si="20"/>
-        <v>1.1276265851314986</v>
+        <f t="shared" ca="1" si="22"/>
+        <v>1.1364560994630302</v>
       </c>
       <c r="T18" s="43">
-        <f>T17-I18</f>
+        <f t="shared" si="12"/>
         <v>3481.1699999999992</v>
       </c>
       <c r="U18" s="43">
@@ -6522,14 +6531,15 @@
         <v>99.7</v>
       </c>
       <c r="I19" s="29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>299.10000000000002</v>
       </c>
       <c r="J19" s="29">
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="K19" s="29">
-        <f t="shared" ref="K19" si="22">J19*I19</f>
+        <f t="shared" ref="K19:K21" si="24">J19*I19</f>
         <v>-299.10000000000002</v>
       </c>
       <c r="L19" s="43" t="s">
@@ -6543,25 +6553,25 @@
       </c>
       <c r="O19" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>-75</v>
+        <v>-70</v>
       </c>
       <c r="P19" s="17">
         <v>0.08</v>
       </c>
       <c r="Q19" s="40">
-        <f t="shared" ca="1" si="8"/>
-        <v>75</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>70</v>
       </c>
       <c r="R19" s="29">
-        <f t="shared" ca="1" si="19"/>
-        <v>1.0266738843331957E-3</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1.1000480543037483E-3</v>
       </c>
       <c r="S19" s="29">
-        <f t="shared" ca="1" si="20"/>
-        <v>1.0990053503540307</v>
+        <f t="shared" ca="1" si="22"/>
+        <v>1.1064412645697368</v>
       </c>
       <c r="T19" s="43">
-        <f>T18-I19</f>
+        <f t="shared" si="12"/>
         <v>3182.0699999999993</v>
       </c>
       <c r="U19" s="43">
@@ -6573,24 +6583,87 @@
       </c>
     </row>
     <row r="20" spans="1:22">
-      <c r="B20" s="1"/>
-      <c r="D20" s="17"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
+      <c r="B20" s="1">
+        <v>44792</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E20" s="44">
+        <v>9</v>
+      </c>
+      <c r="F20" s="44" cm="1">
+        <f t="array" ref="F20">SUMPRODUCT(($C$11:$C$23=C20)*($E$11:$E$23))</f>
+        <v>18</v>
+      </c>
+      <c r="G20">
+        <v>127.73</v>
+      </c>
+      <c r="I20" s="29">
+        <f t="shared" si="19"/>
+        <v>1149.57</v>
+      </c>
+      <c r="J20" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K20" s="29">
+        <f t="shared" si="24"/>
+        <v>1149.57</v>
+      </c>
+      <c r="L20" s="44" t="s">
+        <v>1130</v>
+      </c>
+      <c r="M20" s="44" t="s">
+        <v>138</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="27"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
       <c r="S20" s="17"/>
+      <c r="V20">
+        <f>I20-I15</f>
+        <v>99</v>
+      </c>
     </row>
     <row r="21" spans="1:22">
-      <c r="B21" s="1"/>
-      <c r="D21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="17"/>
+      <c r="B21" s="1">
+        <v>44792</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E21" s="44">
+        <v>35</v>
+      </c>
+      <c r="F21" s="44" cm="1">
+        <f t="array" ref="F21">SUMPRODUCT(($C$11:$C$23=C21)*($E$11:$E$23))</f>
+        <v>105</v>
+      </c>
+      <c r="G21" s="44">
+        <v>33.61</v>
+      </c>
+      <c r="H21" s="42"/>
+      <c r="I21" s="29">
+        <f t="shared" si="19"/>
+        <v>1176.3499999999999</v>
+      </c>
+      <c r="J21" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K21" s="29">
+        <f t="shared" si="24"/>
+        <v>1176.3499999999999</v>
+      </c>
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
       <c r="N21" s="1"/>
@@ -6598,25 +6671,99 @@
       <c r="Q21" s="17"/>
       <c r="R21" s="17"/>
       <c r="S21" s="17"/>
+      <c r="V21" s="44">
+        <f>I21-I12</f>
+        <v>136.14999999999986</v>
+      </c>
     </row>
     <row r="22" spans="1:22">
-      <c r="B22" s="1"/>
-      <c r="J22" s="18"/>
+      <c r="B22" s="1">
+        <v>44792</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="44">
+        <v>35</v>
+      </c>
+      <c r="F22" s="44" cm="1">
+        <f t="array" ref="F22">SUMPRODUCT(($C$11:$C$23=C22)*($E$11:$E$23))</f>
+        <v>105</v>
+      </c>
+      <c r="G22" s="44">
+        <v>33.58</v>
+      </c>
+      <c r="H22" s="42"/>
+      <c r="I22" s="29">
+        <f t="shared" ref="I22" si="25">G22*E22</f>
+        <v>1175.3</v>
+      </c>
+      <c r="J22" s="29">
+        <f t="shared" ref="J22:J23" si="26">IF(D22="BUY",-1,1)</f>
+        <v>-1</v>
+      </c>
+      <c r="K22" s="29">
+        <f t="shared" ref="K22" si="27">J22*I22</f>
+        <v>-1175.3</v>
+      </c>
       <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="27"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
+      <c r="M22" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="N22" s="1">
+        <v>44848</v>
+      </c>
+      <c r="O22" s="40">
+        <f t="shared" ref="O22" ca="1" si="28">$N$9-N22</f>
+        <v>-56</v>
+      </c>
+      <c r="P22" s="29">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q22" s="40">
+        <f ca="1">N22-TODAY()</f>
+        <v>56</v>
+      </c>
+      <c r="R22" s="29">
+        <f t="shared" ref="R22" ca="1" si="29">(1+P22)^(1/Q22)-1</f>
+        <v>7.9724301533745656E-3</v>
+      </c>
+      <c r="S22" s="29">
+        <f t="shared" ref="S22" ca="1" si="30">(1+R22)^92</f>
+        <v>2.0762331738086672</v>
+      </c>
+      <c r="T22" s="44" t="e">
+        <f>C13-I22</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U22" s="44"/>
+      <c r="V22" s="44">
+        <f t="shared" ref="V22" si="31">(I22*(1+P22)-I22)</f>
+        <v>658.16800000000012</v>
+      </c>
     </row>
     <row r="23" spans="1:22">
-      <c r="B23" s="1"/>
-      <c r="D23" s="17"/>
+      <c r="B23" s="1">
+        <v>44792</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>1146</v>
+      </c>
       <c r="E23" s="17"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="17">
+        <v>67.3</v>
+      </c>
       <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
+      <c r="J23" s="29">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
@@ -7061,10 +7208,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="45"/>
+      <c r="B35" s="46"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -7121,10 +7268,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="45"/>
+      <c r="B44" s="46"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -7610,10 +7757,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="45"/>
+      <c r="B38" s="46"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -7670,10 +7817,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="45"/>
+      <c r="B47" s="46"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>
@@ -9056,10 +9203,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="45"/>
+      <c r="B38" s="46"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -9116,10 +9263,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="45"/>
+      <c r="B47" s="46"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -9442,10 +9589,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="45"/>
+      <c r="B35" s="46"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -9502,10 +9649,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="45"/>
+      <c r="B44" s="46"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -10002,10 +10149,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="45"/>
+      <c r="B15" s="46"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -10062,10 +10209,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="45"/>
+      <c r="B24" s="46"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -10380,10 +10527,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="45"/>
+      <c r="B32" s="46"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -10440,10 +10587,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="45"/>
+      <c r="B41" s="46"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -14174,10 +14321,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="45"/>
+      <c r="B35" s="46"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -14234,10 +14381,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="45"/>
+      <c r="B44" s="46"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -14565,10 +14712,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="45"/>
+      <c r="B35" s="46"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -14625,10 +14772,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="45"/>
+      <c r="B44" s="46"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -15768,10 +15915,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="45"/>
+      <c r="B35" s="46"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -15828,10 +15975,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="45"/>
+      <c r="B44" s="46"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -16444,10 +16591,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="44" t="s">
+      <c r="A63" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="45"/>
+      <c r="B63" s="46"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -16504,10 +16651,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="44" t="s">
+      <c r="A72" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="45"/>
+      <c r="B72" s="46"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -16967,10 +17114,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="45"/>
+      <c r="B32" s="46"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -17027,10 +17174,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="45"/>
+      <c r="B41" s="46"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -18118,10 +18265,10 @@
       <c r="A31" s="21"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="45"/>
+      <c r="B32" s="46"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -18178,10 +18325,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="45"/>
+      <c r="B41" s="46"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>

</xml_diff>

<commit_message>
backtest algorithm implemented with cluster parallel processing
</commit_message>
<xml_diff>
--- a/code/Screener/data/interim/record.xlsx
+++ b/code/Screener/data/interim/record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\wiki\wiki\dev\python\Python-Stock\code\Screener\data\interim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF43118-C03B-4E13-A526-ECFC04D80328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B0EC86-0193-4471-95C8-64094C68B62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{785F8A36-E86A-4BD6-94E8-FC2E8B05B64B}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="1148">
   <si>
     <t>MCK</t>
   </si>
@@ -3513,6 +3513,9 @@
   </si>
   <si>
     <t>Sell</t>
+  </si>
+  <si>
+    <t>ATEN</t>
   </si>
 </sst>
 </file>
@@ -3627,7 +3630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3715,6 +3718,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5807,7 +5811,7 @@
   <dimension ref="A3:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5842,7 +5846,7 @@
       </c>
       <c r="E4" s="1">
         <f ca="1">TODAY()</f>
-        <v>44792</v>
+        <v>44793</v>
       </c>
       <c r="G4" t="s">
         <v>1142</v>
@@ -5882,7 +5886,7 @@
       </c>
       <c r="N9" s="1">
         <f ca="1">TODAY()</f>
-        <v>44792</v>
+        <v>44793</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>1050</v>
@@ -6013,22 +6017,22 @@
       </c>
       <c r="O12" s="40">
         <f t="shared" ref="O12:O19" ca="1" si="2">$N$9-N12</f>
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="P12" s="29">
         <v>0.56000000000000005</v>
       </c>
       <c r="Q12" s="40">
         <f ca="1">N12-TODAY()</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R12" s="29">
         <f t="shared" ref="R12" ca="1" si="3">(1+P12)^(1/Q12)-1</f>
-        <v>7.9724301533745656E-3</v>
+        <v>8.1179702205613768E-3</v>
       </c>
       <c r="S12" s="29">
         <f t="shared" ref="S12" ca="1" si="4">(1+R12)^92</f>
-        <v>2.0762331738086672</v>
+        <v>2.1039953841313968</v>
       </c>
       <c r="T12">
         <f>C3-I12</f>
@@ -6088,25 +6092,25 @@
       </c>
       <c r="O13" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="P13">
         <v>0.18</v>
       </c>
       <c r="Q13" s="40">
         <f t="shared" ref="Q13:Q19" ca="1" si="9">N13-TODAY()</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R13" s="29">
         <f t="shared" ref="R13" ca="1" si="10">(1+P13)^(1/Q13)-1</f>
-        <v>2.95998710913703E-3</v>
+        <v>3.0138860765300812E-3</v>
       </c>
       <c r="S13" s="29">
         <f t="shared" ref="S13:S14" ca="1" si="11">(1+R13)^92</f>
-        <v>1.3124775065877488</v>
+        <v>1.3189823803042053</v>
       </c>
       <c r="T13" s="39">
-        <f t="shared" ref="T13:T19" si="12">T12-I13</f>
+        <f t="shared" ref="T13:T24" si="12">T12-I13</f>
         <v>7829.9999999999991</v>
       </c>
       <c r="V13" s="39">
@@ -6132,7 +6136,7 @@
       </c>
       <c r="F14" s="39" cm="1">
         <f t="array" ref="F14">SUMPRODUCT(($C$11:$C$23=C14)*($E$11:$E$23))</f>
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="G14">
         <v>71.94</v>
@@ -6163,22 +6167,22 @@
       </c>
       <c r="O14" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="Q14" s="40">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="29" t="e">
+        <v>-1</v>
+      </c>
+      <c r="R14" s="29">
         <f t="shared" ref="R14" ca="1" si="14">(1+P14)^(1/Q14)-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S14" s="29" t="e">
+        <v>-8.6757990867579848E-2</v>
+      </c>
+      <c r="S14" s="29">
         <f t="shared" ca="1" si="11"/>
-        <v>#DIV/0!</v>
+        <v>2.3653806285002716E-4</v>
       </c>
       <c r="T14" s="39">
         <f t="shared" si="12"/>
@@ -6241,22 +6245,22 @@
       </c>
       <c r="O15" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15" s="41">
         <v>0.04</v>
       </c>
       <c r="Q15" s="40">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="29" t="e">
+        <v>-1</v>
+      </c>
+      <c r="R15" s="29">
         <f t="shared" ref="R15" ca="1" si="15">(1+P15)^(1/Q15)-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S15" s="29" t="e">
+        <v>-3.8461538461538547E-2</v>
+      </c>
+      <c r="S15" s="29">
         <f t="shared" ref="S15" ca="1" si="16">(1+R15)^92</f>
-        <v>#DIV/0!</v>
+        <v>2.7097722096693963E-2</v>
       </c>
       <c r="T15" s="41">
         <f t="shared" si="12"/>
@@ -6319,22 +6323,22 @@
       </c>
       <c r="O16" s="40">
         <f t="shared" ca="1" si="2"/>
-        <v>-63</v>
+        <v>-62</v>
       </c>
       <c r="P16" s="17">
         <v>0.128</v>
       </c>
       <c r="Q16" s="40">
         <f t="shared" ca="1" si="9"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R16" s="29">
         <f t="shared" ref="R16" ca="1" si="17">(1+P16)^(1/Q16)-1</f>
-        <v>1.9136724380177661E-3</v>
+        <v>1.9445681134357962E-3</v>
       </c>
       <c r="S16" s="29">
         <f t="shared" ref="S16" ca="1" si="18">(1+R16)^92</f>
-        <v>1.192306445036563</v>
+        <v>1.1956937366792555</v>
       </c>
       <c r="T16" s="41">
         <f t="shared" si="12"/>
@@ -6397,22 +6401,22 @@
       </c>
       <c r="O17" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="P17" s="41">
         <v>0.128</v>
       </c>
       <c r="Q17" s="40">
         <f t="shared" ca="1" si="9"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R17" s="29">
         <f t="shared" ref="R17:R19" ca="1" si="21">(1+P17)^(1/Q17)-1</f>
-        <v>2.1531388435505061E-3</v>
+        <v>2.1923297041173129E-3</v>
       </c>
       <c r="S17" s="29">
         <f t="shared" ref="S17:S19" ca="1" si="22">(1+R17)^92</f>
-        <v>1.2188110360169528</v>
+        <v>1.2232039014177503</v>
       </c>
       <c r="T17" s="41">
         <f t="shared" si="12"/>
@@ -6475,22 +6479,22 @@
       </c>
       <c r="O18" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>-77</v>
+        <v>-76</v>
       </c>
       <c r="P18">
         <v>0.113</v>
       </c>
       <c r="Q18" s="40">
         <f t="shared" ca="1" si="9"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R18" s="29">
         <f t="shared" ca="1" si="21"/>
-        <v>1.3913445852586914E-3</v>
+        <v>1.4096646483165998E-3</v>
       </c>
       <c r="S18" s="29">
         <f t="shared" ca="1" si="22"/>
-        <v>1.1364560994630302</v>
+        <v>1.1383704663729126</v>
       </c>
       <c r="T18" s="43">
         <f t="shared" si="12"/>
@@ -6553,22 +6557,22 @@
       </c>
       <c r="O19" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>-70</v>
+        <v>-69</v>
       </c>
       <c r="P19" s="17">
         <v>0.08</v>
       </c>
       <c r="Q19" s="40">
         <f t="shared" ca="1" si="9"/>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R19" s="29">
         <f t="shared" ca="1" si="21"/>
-        <v>1.1000480543037483E-3</v>
+        <v>1.1159996724827703E-3</v>
       </c>
       <c r="S19" s="29">
         <f t="shared" ca="1" si="22"/>
-        <v>1.1064412645697368</v>
+        <v>1.1080644134465059</v>
       </c>
       <c r="T19" s="43">
         <f t="shared" si="12"/>
@@ -6626,6 +6630,10 @@
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
       <c r="S20" s="17"/>
+      <c r="T20" s="45">
+        <f t="shared" si="12"/>
+        <v>2032.4999999999993</v>
+      </c>
       <c r="V20">
         <f>I20-I15</f>
         <v>99</v>
@@ -6671,6 +6679,10 @@
       <c r="Q21" s="17"/>
       <c r="R21" s="17"/>
       <c r="S21" s="17"/>
+      <c r="T21" s="45">
+        <f t="shared" si="12"/>
+        <v>856.14999999999941</v>
+      </c>
       <c r="V21" s="44">
         <f>I21-I12</f>
         <v>136.14999999999986</v>
@@ -6698,11 +6710,11 @@
       </c>
       <c r="H22" s="42"/>
       <c r="I22" s="29">
-        <f t="shared" ref="I22" si="25">G22*E22</f>
+        <f t="shared" ref="I22:I24" si="25">G22*E22</f>
         <v>1175.3</v>
       </c>
       <c r="J22" s="29">
-        <f t="shared" ref="J22:J23" si="26">IF(D22="BUY",-1,1)</f>
+        <f t="shared" ref="J22:J24" si="26">IF(D22="BUY",-1,1)</f>
         <v>-1</v>
       </c>
       <c r="K22" s="29">
@@ -6718,26 +6730,26 @@
       </c>
       <c r="O22" s="40">
         <f t="shared" ref="O22" ca="1" si="28">$N$9-N22</f>
-        <v>-56</v>
+        <v>-55</v>
       </c>
       <c r="P22" s="29">
         <v>0.56000000000000005</v>
       </c>
       <c r="Q22" s="40">
         <f ca="1">N22-TODAY()</f>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R22" s="29">
         <f t="shared" ref="R22" ca="1" si="29">(1+P22)^(1/Q22)-1</f>
-        <v>7.9724301533745656E-3</v>
+        <v>8.1179702205613768E-3</v>
       </c>
       <c r="S22" s="29">
         <f t="shared" ref="S22" ca="1" si="30">(1+R22)^92</f>
-        <v>2.0762331738086672</v>
-      </c>
-      <c r="T22" s="44" t="e">
-        <f>C13-I22</f>
-        <v>#VALUE!</v>
+        <v>2.1039953841313968</v>
+      </c>
+      <c r="T22" s="45">
+        <f t="shared" si="12"/>
+        <v>-319.15000000000055</v>
       </c>
       <c r="U22" s="44"/>
       <c r="V22" s="44">
@@ -6746,6 +6758,7 @@
       </c>
     </row>
     <row r="23" spans="1:22">
+      <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>44792</v>
       </c>
@@ -6755,7 +6768,12 @@
       <c r="D23" s="17" t="s">
         <v>1146</v>
       </c>
-      <c r="E23" s="17"/>
+      <c r="E23" s="45">
+        <v>35</v>
+      </c>
+      <c r="F23" s="45">
+        <v>0</v>
+      </c>
       <c r="G23" s="17">
         <v>67.3</v>
       </c>
@@ -6772,20 +6790,74 @@
       <c r="Q23" s="17"/>
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
+      <c r="T23" s="45">
+        <f t="shared" si="12"/>
+        <v>-319.15000000000055</v>
+      </c>
     </row>
     <row r="24" spans="1:22">
-      <c r="B24" s="1"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="A24" s="1">
+        <v>44792</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44793</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="18">
+        <v>16</v>
+      </c>
+      <c r="F24" s="45" cm="1">
+        <f t="array" ref="F24">SUMPRODUCT(($C$11:$C$23=C24)*($E$11:$E$23))</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>16.21</v>
+      </c>
+      <c r="H24" s="38">
+        <v>16.04</v>
+      </c>
+      <c r="I24" s="29">
+        <f t="shared" si="25"/>
+        <v>259.36</v>
+      </c>
+      <c r="J24" s="29">
+        <f t="shared" si="26"/>
+        <v>-1</v>
+      </c>
       <c r="K24" s="26"/>
-      <c r="N24" s="1"/>
+      <c r="N24" s="1">
+        <v>44876</v>
+      </c>
       <c r="O24" s="27"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
+      <c r="P24" s="26">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q24" s="40">
+        <f ca="1">N24-TODAY()</f>
+        <v>83</v>
+      </c>
+      <c r="R24" s="29">
+        <f t="shared" ref="R24" ca="1" si="32">(1+P24)^(1/Q24)-1</f>
+        <v>1.5799004937511185E-3</v>
+      </c>
+      <c r="S24" s="29">
+        <f t="shared" ref="S24" ca="1" si="33">(1+R24)^92</f>
+        <v>1.1563125969500117</v>
+      </c>
+      <c r="T24" s="45">
+        <f t="shared" si="12"/>
+        <v>-578.51000000000056</v>
+      </c>
+      <c r="U24" s="45"/>
+      <c r="V24" s="45">
+        <f t="shared" ref="V24" si="34">(I24*(1+P24)-I24)</f>
+        <v>36.310400000000016</v>
+      </c>
     </row>
     <row r="25" spans="1:22">
       <c r="B25" s="1"/>
@@ -7208,10 +7280,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="47"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -7268,10 +7340,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="46"/>
+      <c r="B44" s="47"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -7757,10 +7829,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="46"/>
+      <c r="B38" s="47"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6"/>
@@ -7817,10 +7889,10 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="46"/>
+      <c r="B47" s="47"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6"/>
@@ -9203,10 +9275,10 @@
       <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="46"/>
+      <c r="B38" s="47"/>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="6"/>
@@ -9263,10 +9335,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="46"/>
+      <c r="B47" s="47"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
@@ -9589,10 +9661,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="47"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -9649,10 +9721,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="46"/>
+      <c r="B44" s="47"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -10149,10 +10221,10 @@
       <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="46"/>
+      <c r="B15" s="47"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6"/>
@@ -10209,10 +10281,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="46"/>
+      <c r="B24" s="47"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6"/>
@@ -10527,10 +10599,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="46"/>
+      <c r="B32" s="47"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -10587,10 +10659,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="46"/>
+      <c r="B41" s="47"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -14321,10 +14393,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="47"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -14381,10 +14453,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="46"/>
+      <c r="B44" s="47"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -14712,10 +14784,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="47"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -14772,10 +14844,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="46"/>
+      <c r="B44" s="47"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -15915,10 +15987,10 @@
       <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="47"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="6"/>
@@ -15975,10 +16047,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="46"/>
+      <c r="B44" s="47"/>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="6"/>
@@ -16591,10 +16663,10 @@
       <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="45" t="s">
+      <c r="A63" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="46"/>
+      <c r="B63" s="47"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="6"/>
@@ -16651,10 +16723,10 @@
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="45" t="s">
+      <c r="A72" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B72" s="46"/>
+      <c r="B72" s="47"/>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6"/>
@@ -17114,10 +17186,10 @@
       <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="46"/>
+      <c r="B32" s="47"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6"/>
@@ -17174,10 +17246,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="46"/>
+      <c r="B41" s="47"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="6"/>
@@ -18265,10 +18337,10 @@
       <c r="A31" s="21"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="46"/>
+      <c r="B32" s="47"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="12"/>
@@ -18325,10 +18397,10 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="47" t="s">
+      <c r="A41" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="46"/>
+      <c r="B41" s="47"/>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="12"/>

</xml_diff>